<commit_message>
process updated for USA process
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yazmin\AutomationProcesses\cinepolis\CinepolisUSA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44A782A-7AC7-4D15-A7CA-D907CD42E55B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF358659-A7C0-4A1A-8472-DD3E2CE77EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
   <si>
     <t>Name</t>
   </si>
@@ -193,13 +193,73 @@
   </si>
   <si>
     <t>BDMHEfilePath</t>
+  </si>
+  <si>
+    <t>DataNoBelongToCurrentWeekMailSubject</t>
+  </si>
+  <si>
+    <t>Notification- Data doesn't belong to this week</t>
+  </si>
+  <si>
+    <t>DataNoBelongToCurrentWeekMailBody</t>
+  </si>
+  <si>
+    <t>MailTo</t>
+  </si>
+  <si>
+    <t>manindersinghbisht77@gmail.com</t>
+  </si>
+  <si>
+    <t>MailCC</t>
+  </si>
+  <si>
+    <t>InputFileExceptionSubject</t>
+  </si>
+  <si>
+    <t>Error- Input file Notification</t>
+  </si>
+  <si>
+    <t>InputFileExceptionbody</t>
+  </si>
+  <si>
+    <t>Notification- Not All file Got downloaded</t>
+  </si>
+  <si>
+    <t>downloadFileExceptionSubject</t>
+  </si>
+  <si>
+    <t>downloadFileExceptionbody</t>
+  </si>
+  <si>
+    <t>Dear Team&lt;br/&gt;
+Please find the below data which does not belong to current week.&lt;br/&gt;
+[Nothisweekdatatable]&lt;br&gt;
+Also let us know if anything is required&lt;br/&gt;
+Thank you,&lt;br/&gt;
+**********************This is system generated E-Mail, please do not respond on this************</t>
+  </si>
+  <si>
+    <t>Dear Team&lt;br/&gt;
+There is a error in Cinepolish USA run, below is the detail of error&lt;br/&gt;
+[error]&lt;br/&gt;
+Also let us know if anything is required&lt;br/&gt;
+Thank you,&lt;br/&gt;
+**********************This is system generated E-Mail, please do not respond on this************</t>
+  </si>
+  <si>
+    <t>Dear Team&lt;br/&gt;
+There is a error in Cinepos USA process run, below is the detail of error&lt;br/&gt;
+Not all required files got downloaded from FTP&lt;br/&gt;
+Also let us know if anything is required&lt;br/&gt;
+Thank you,&lt;br/&gt;
+**********************This is system generated E-Mail, please do not respond on this************</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -321,6 +381,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -339,10 +405,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -383,8 +450,15 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -699,7 +773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -965,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1041,21 +1115,77 @@
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="B5" s="13"/>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B7" s="2"/>
+      <c r="A7" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B8" s="9"/>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="26"/>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="24"/>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>71</v>
+      </c>
+    </row>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -2020,8 +2150,11 @@
     <row r="978" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{B1018490-FE45-47D5-A281-E8373B4E93A6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
changes in config file done from my end
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\CinepolisUSA\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yazmin\AutomationProcesses\cinepolis\CinepolisUSA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADDA75E-34D9-4446-98E9-2C6E123D250C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE75BC6-E882-49E8-B863-824A4AF8406E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
   <si>
     <t>Name</t>
   </si>
@@ -93,9 +93,15 @@
     <t>InputnonPartnerFilePath</t>
   </si>
   <si>
+    <t>/Planeacion/0.Envios TS 2021/1 Directorio</t>
+  </si>
+  <si>
     <t>input file path for non partner file</t>
   </si>
   <si>
+    <t>BD_ENCUESTA_LARGA_GULF_Tradicio</t>
+  </si>
+  <si>
     <t>InputSheetName</t>
   </si>
   <si>
@@ -105,6 +111,15 @@
     <t>InputVIPSheetName</t>
   </si>
   <si>
+    <t>LUXURY</t>
+  </si>
+  <si>
+    <t>TRADICIONAL</t>
+  </si>
+  <si>
+    <t>BD_ENCUESTA_LARGA_GULF_VIP_Sema</t>
+  </si>
+  <si>
     <t>DirectirioFilePath</t>
   </si>
   <si>
@@ -115,6 +130,33 @@
   </si>
   <si>
     <t>DirectorioSheetName</t>
+  </si>
+  <si>
+    <t>España</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/33 Envio Semana 31/ESPAÑA/TRADICIONAL</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/33 Envio Semana 31/ESPAÑA/LUXURY</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/32 Envio Semana 32</t>
+  </si>
+  <si>
+    <t>REPORTE_ESTUDIOC_CHILE_SEM_49</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/32 Envio Semana 32/CHILE/Base de Datos</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/32 Envio Semana 32/CHILE/Base de Datos/Exportadas</t>
+  </si>
+  <si>
+    <t>CHILE</t>
+  </si>
+  <si>
+    <t>/Planning/0.Shipping TS 2021/1 Directory</t>
   </si>
   <si>
     <t>BDLuxuryfilePath</t>
@@ -211,36 +253,6 @@
 Also let us know if anything is required&lt;br/&gt;
 Thank you,&lt;br/&gt;
 **********************This is system generated E-Mail, please do not respond on this************</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/USA/Base de Datos</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/USA/LUXURY</t>
-  </si>
-  <si>
-    <t>BD_USA_Luxury_Semana_X_X_X</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/USA/PREMIUM</t>
-  </si>
-  <si>
-    <t>BD_USA_Premium_Semana_XX_XX_XXX</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/USA/MHE</t>
-  </si>
-  <si>
-    <t>BD_USA_MHE_Semana_XX_XX_XXX</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/USA/Base de Datos/Exportadas</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/1 Directorio</t>
   </si>
 </sst>
 </file>
@@ -761,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -787,31 +799,35 @@
         <v>22</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75">
       <c r="A4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="21"/>
+        <v>27</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="15.75">
       <c r="A5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="21"/>
+        <v>28</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="15.75">
       <c r="A6" s="2"/>
@@ -819,18 +835,18 @@
     </row>
     <row r="7" spans="1:3" ht="15.75">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -839,18 +855,18 @@
     </row>
     <row r="10" spans="1:3" ht="15.75">
       <c r="A10" s="2" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -859,18 +875,18 @@
     </row>
     <row r="13" spans="1:3" ht="15.75">
       <c r="A13" s="2" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75">
@@ -878,7 +894,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -891,15 +907,15 @@
     </row>
     <row r="19" spans="1:2" ht="15.75">
       <c r="A19" s="2" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
         <v>14</v>
@@ -907,15 +923,15 @@
     </row>
     <row r="22" spans="1:2" ht="15.75">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
         <v>14</v>
@@ -926,15 +942,15 @@
     </row>
     <row r="25" spans="1:2" ht="15.75">
       <c r="A25" s="2" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
         <v>14</v>
@@ -945,18 +961,18 @@
     </row>
     <row r="28" spans="1:2" ht="15.75">
       <c r="A28" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -996,18 +1012,18 @@
     </row>
     <row r="36" spans="1:2" ht="15.75">
       <c r="A36" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B36" s="23" t="s">
-        <v>67</v>
+        <v>34</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75">
       <c r="A37" s="21" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1023,7 +1039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1101,18 +1117,18 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="24" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="24" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1121,15 +1137,15 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="24" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="24" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B10" s="24"/>
     </row>
@@ -1139,35 +1155,35 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="24" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="24" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="24" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="24" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
input file name standardise
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\CinepolisUSA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DD1227-03BF-44A2-96F7-CACD240DF343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D887D5-A156-4DC8-92E0-A49FDD0FD25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
   <si>
     <t>Name</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>/Planeacion/0.Envios TS/1 Directorio</t>
+  </si>
+  <si>
+    <t>Key words in filename</t>
+  </si>
+  <si>
+    <t>Report and USA</t>
   </si>
 </sst>
 </file>
@@ -762,19 +768,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="84.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75">
+    <row r="1" spans="1:4" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -784,8 +791,11 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75">
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -795,8 +805,11 @@
       <c r="C2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -804,7 +817,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75">
+    <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -812,7 +825,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75">
+    <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -820,11 +833,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75">
+    <row r="6" spans="1:4" ht="15.75">
       <c r="A6" s="2"/>
       <c r="B6" s="21"/>
     </row>
-    <row r="7" spans="1:3" ht="15.75">
+    <row r="7" spans="1:4" ht="15.75">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -832,7 +845,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
@@ -840,11 +853,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9" s="2"/>
       <c r="B9" s="22"/>
     </row>
-    <row r="10" spans="1:3" ht="15.75">
+    <row r="10" spans="1:4" ht="15.75">
       <c r="A10" s="2" t="s">
         <v>41</v>
       </c>
@@ -852,7 +865,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>42</v>
       </c>
@@ -860,11 +873,11 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:4">
       <c r="A12" s="2"/>
       <c r="B12" s="22"/>
     </row>
-    <row r="13" spans="1:3" ht="15.75">
+    <row r="13" spans="1:4" ht="15.75">
       <c r="A13" s="2" t="s">
         <v>44</v>
       </c>
@@ -872,7 +885,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
         <v>43</v>
       </c>
@@ -880,7 +893,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75">
+    <row r="16" spans="1:4" ht="15.75">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
changes in input file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\CinepolisUSA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D887D5-A156-4DC8-92E0-A49FDD0FD25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F2BE62-E87E-4631-A75D-3869FCC50D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="72">
   <si>
     <t>Name</t>
   </si>
@@ -252,14 +252,14 @@
     <t>Key words in filename</t>
   </si>
   <si>
-    <t>Report and USA</t>
+    <t>Report, USA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -387,6 +387,13 @@
       <color theme="10"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -409,7 +416,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -453,6 +460,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -771,7 +779,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -791,7 +799,7 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="27" t="s">
         <v>70</v>
       </c>
     </row>
@@ -805,7 +813,7 @@
       <c r="C2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>

<commit_message>
correct name implimented in input file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\CinepolisUSA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F2BE62-E87E-4631-A75D-3869FCC50D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AD6E2A-691B-4831-923E-9427F02E1423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="750" windowWidth="16140" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -253,6 +253,12 @@
   </si>
   <si>
     <t>Report, USA</t>
+  </si>
+  <si>
+    <t>CorrectnameFilePath</t>
+  </si>
+  <si>
+    <t>CorrectSheetName</t>
   </si>
 </sst>
 </file>
@@ -776,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1036,6 +1042,16 @@
       </c>
       <c r="B37" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
process updated for current week data
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\CinepolisUSA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AD6E2A-691B-4831-923E-9427F02E1423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D664474C-40D2-4276-9CBB-0BAD9C32BBF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="750" windowWidth="16140" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="16140" windowHeight="10170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="77">
   <si>
     <t>Name</t>
   </si>
@@ -259,6 +259,15 @@
   </si>
   <si>
     <t>CorrectSheetName</t>
+  </si>
+  <si>
+    <t>WorkingStartDate</t>
+  </si>
+  <si>
+    <t>dd/MM/yyyy</t>
+  </si>
+  <si>
+    <t>WorkingEndDate</t>
   </si>
 </sst>
 </file>
@@ -422,7 +431,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -467,6 +476,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -784,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1067,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1214,22 +1225,42 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="28">
+        <v>44599</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="28">
+        <v>44605</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
code updated for the USA testing
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\CinepolisUSA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D664474C-40D2-4276-9CBB-0BAD9C32BBF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6DF521-0599-44BD-B522-E8451E4DF802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="16140" windowHeight="10170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="77">
   <si>
     <t>Name</t>
   </si>
@@ -109,12 +109,6 @@
   </si>
   <si>
     <t>TRADICIONAL</t>
-  </si>
-  <si>
-    <t>DirectirioFilePath</t>
-  </si>
-  <si>
-    <t>DirectirioSheetName</t>
   </si>
   <si>
     <t>DirectorioFilePath</t>
@@ -219,30 +213,15 @@
 **********************This is system generated E-Mail, please do not respond on this************</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS/2022/05 Envio Semana 05/USA/Base de Datos</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/05 Envio Semana 05/USA/LUXURY</t>
-  </si>
-  <si>
     <t>BD_USA_Luxury_Semana_X_X_X</t>
   </si>
   <si>
     <t>BD_USA_Premium_Semana_XX_XX_XXX</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS/2022/05 Envio Semana 05/USA/PREMIUM</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/05 Envio Semana 05/USA/MHE</t>
-  </si>
-  <si>
     <t>BD_USA_MHE_Semana_XX_XX_XXX</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS/2022/05 Envio Semana 05/USA/Base de Datos/Exportadas</t>
-  </si>
-  <si>
     <t>USA</t>
   </si>
   <si>
@@ -268,6 +247,27 @@
   </si>
   <si>
     <t>WorkingEndDate</t>
+  </si>
+  <si>
+    <t>Hoja</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/USA/Base de Datos</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/USA/LUXURY</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/USA/PREMIUM</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/USA/MHE</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/USA/Base de Datos/Exportadas</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/1 Directorio/Correcciones</t>
   </si>
 </sst>
 </file>
@@ -793,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -804,6 +804,7 @@
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="84.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75">
@@ -817,7 +818,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75">
@@ -825,13 +826,13 @@
         <v>22</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -864,18 +865,18 @@
     </row>
     <row r="7" spans="1:4" ht="15.75">
       <c r="A7" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -884,18 +885,18 @@
     </row>
     <row r="10" spans="1:4" ht="15.75">
       <c r="A10" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -904,18 +905,18 @@
     </row>
     <row r="13" spans="1:4" ht="15.75">
       <c r="A13" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75">
@@ -923,7 +924,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -936,15 +937,15 @@
     </row>
     <row r="19" spans="1:2" ht="15.75">
       <c r="A19" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
         <v>14</v>
@@ -952,15 +953,15 @@
     </row>
     <row r="22" spans="1:2" ht="15.75">
       <c r="A22" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
         <v>14</v>
@@ -971,15 +972,15 @@
     </row>
     <row r="25" spans="1:2" ht="15.75">
       <c r="A25" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
         <v>14</v>
@@ -989,85 +990,75 @@
       <c r="A27" s="2"/>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" t="s">
-        <v>69</v>
-      </c>
+      <c r="A28" s="2"/>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" t="s">
-        <v>68</v>
+        <v>9</v>
+      </c>
+      <c r="B29" s="16">
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="2"/>
+      <c r="A30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="16">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32" s="19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33" s="20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="4" t="s">
+      <c r="A32" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B32" s="20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15.75">
-      <c r="A36" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="15.75">
-      <c r="A37" s="21" t="s">
-        <v>32</v>
+    <row r="34" spans="1:2" ht="15.75">
+      <c r="A34" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75">
+      <c r="A35" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>65</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s">
-        <v>73</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B32" r:id="rId1" xr:uid="{58EC0946-E8B4-4BDB-80EA-7ED2F2D369BC}"/>
+    <hyperlink ref="B30" r:id="rId1" xr:uid="{58EC0946-E8B4-4BDB-80EA-7ED2F2D369BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1078,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:C19"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1156,18 +1147,18 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1176,15 +1167,15 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B10" s="23"/>
     </row>
@@ -1194,58 +1185,58 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="23" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B18" s="28">
         <v>44599</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" s="23" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B19" s="28">
         <v>44605</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>